<commit_message>
commit taxillasuite to master
</commit_message>
<xml_diff>
--- a/TaxillaSuite/InputFile/inbound.xlsx
+++ b/TaxillaSuite/InputFile/inbound.xlsx
@@ -32,7 +32,7 @@
     <t xml:space="preserve">f3</t>
   </si>
   <si>
-    <t xml:space="preserve">test80</t>
+    <t xml:space="preserve">test83</t>
   </si>
   <si>
     <t xml:space="preserve">test1</t>
@@ -53,7 +53,7 @@
     <t xml:space="preserve">f7</t>
   </si>
   <si>
-    <t xml:space="preserve"> test80</t>
+    <t xml:space="preserve"> test83</t>
   </si>
   <si>
     <t xml:space="preserve">111</t>

</xml_diff>